<commit_message>
clean code with new pickles + updates on plots
</commit_message>
<xml_diff>
--- a/results/basic/percentages.xlsx
+++ b/results/basic/percentages.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="day1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="day2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="day3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="day4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="day5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="day6" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="day1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="day2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="day3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="day4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="day5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="day6" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>85.71428571428571</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>14.28571428571428</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -608,7 +608,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -699,7 +699,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
@@ -729,7 +729,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>60</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="3">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="6">
@@ -900,7 +900,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>61.53846153846154</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.692307692307693</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -981,7 +981,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.692307692307693</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7.692307692307693</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7.692307692307693</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1021,7 +1021,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7.692307692307693</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="3">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>